<commit_message>
Avances denoiser, sigue sin estar del todo, ejemplos muy basicos funcionan
</commit_message>
<xml_diff>
--- a/AlejandroAlonso/results/excels/tracking_short_AlejandroAlonso.xlsx
+++ b/AlejandroAlonso/results/excels/tracking_short_AlejandroAlonso.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t xml:space="preserve">Sistema:</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t xml:space="preserve">Bola num 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bola num 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bola num 6</t>
   </si>
   <si>
     <t xml:space="preserve">X</t>
@@ -165,7 +171,7 @@
   <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="1" sqref="H5:I68 F7"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="1" sqref="N12:O15 F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -210,10 +216,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5:I68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -238,32 +244,62 @@
         <v>9</v>
       </c>
       <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,6 +531,12 @@
       <c r="I12" s="1" t="n">
         <v>1185</v>
       </c>
+      <c r="N12" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -518,6 +560,12 @@
       <c r="I13" s="1" t="n">
         <v>1154</v>
       </c>
+      <c r="N13" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -541,6 +589,12 @@
       <c r="I14" s="1" t="n">
         <v>1078</v>
       </c>
+      <c r="N14" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -564,6 +618,12 @@
       <c r="I15" s="1" t="n">
         <v>1011</v>
       </c>
+      <c r="N15" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -730,12 +790,6 @@
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="D23" s="1" t="n">
-        <v>529</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>1088</v>
-      </c>
       <c r="F23" s="1" t="n">
         <v>637</v>
       </c>
@@ -747,18 +801,18 @@
       </c>
       <c r="I23" s="1" t="n">
         <v>780</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <v>529</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>1088</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="D24" s="1" t="n">
-        <v>527</v>
-      </c>
-      <c r="E24" s="1" t="n">
-        <v>1099</v>
-      </c>
       <c r="F24" s="1" t="n">
         <v>620</v>
       </c>
@@ -770,18 +824,18 @@
       </c>
       <c r="I24" s="1" t="n">
         <v>779</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <v>527</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>1099</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="D25" s="1" t="n">
-        <v>525</v>
-      </c>
-      <c r="E25" s="1" t="n">
-        <v>1112</v>
-      </c>
       <c r="F25" s="1" t="n">
         <v>605</v>
       </c>
@@ -793,18 +847,18 @@
       </c>
       <c r="I25" s="1" t="n">
         <v>785</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <v>525</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>1112</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="D26" s="1" t="n">
-        <v>523</v>
-      </c>
-      <c r="E26" s="1" t="n">
-        <v>1131</v>
-      </c>
       <c r="F26" s="1" t="n">
         <v>592</v>
       </c>
@@ -816,18 +870,18 @@
       </c>
       <c r="I26" s="1" t="n">
         <v>792</v>
+      </c>
+      <c r="J26" s="1" t="n">
+        <v>523</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>1131</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="D27" s="1" t="n">
-        <v>521</v>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>1152</v>
-      </c>
       <c r="F27" s="1" t="n">
         <v>585</v>
       </c>
@@ -839,18 +893,18 @@
       </c>
       <c r="I27" s="1" t="n">
         <v>803</v>
+      </c>
+      <c r="J27" s="1" t="n">
+        <v>521</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>1152</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="D28" s="1" t="n">
-        <v>518</v>
-      </c>
-      <c r="E28" s="1" t="n">
-        <v>1176</v>
-      </c>
       <c r="F28" s="1" t="n">
         <v>580</v>
       </c>
@@ -862,18 +916,18 @@
       </c>
       <c r="I28" s="1" t="n">
         <v>823</v>
+      </c>
+      <c r="J28" s="1" t="n">
+        <v>518</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>1176</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="D29" s="1" t="n">
-        <v>524</v>
-      </c>
-      <c r="E29" s="1" t="n">
-        <v>1183</v>
-      </c>
       <c r="F29" s="1" t="n">
         <v>575</v>
       </c>
@@ -885,18 +939,18 @@
       </c>
       <c r="I29" s="1" t="n">
         <v>849</v>
+      </c>
+      <c r="J29" s="1" t="n">
+        <v>524</v>
+      </c>
+      <c r="K29" s="1" t="n">
+        <v>1183</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="D30" s="1" t="n">
-        <v>526</v>
-      </c>
-      <c r="E30" s="1" t="n">
-        <v>1204</v>
-      </c>
       <c r="F30" s="1" t="n">
         <v>571</v>
       </c>
@@ -908,18 +962,18 @@
       </c>
       <c r="I30" s="1" t="n">
         <v>876</v>
+      </c>
+      <c r="J30" s="1" t="n">
+        <v>526</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>1204</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="D31" s="1" t="n">
-        <v>528</v>
-      </c>
-      <c r="E31" s="1" t="n">
-        <v>1225</v>
-      </c>
       <c r="F31" s="1" t="n">
         <v>564</v>
       </c>
@@ -931,18 +985,18 @@
       </c>
       <c r="I31" s="1" t="n">
         <v>904</v>
+      </c>
+      <c r="J31" s="1" t="n">
+        <v>528</v>
+      </c>
+      <c r="K31" s="1" t="n">
+        <v>1225</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D32" s="1" t="n">
-        <v>532</v>
-      </c>
-      <c r="E32" s="1" t="n">
-        <v>1239</v>
-      </c>
       <c r="F32" s="1" t="n">
         <v>556</v>
       </c>
@@ -954,28 +1008,34 @@
       </c>
       <c r="I32" s="1" t="n">
         <v>936</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>532</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <v>1239</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="D33" s="1" t="n">
-        <v>538</v>
-      </c>
-      <c r="E33" s="1" t="n">
-        <v>1241</v>
-      </c>
       <c r="F33" s="1" t="n">
         <v>546</v>
       </c>
       <c r="G33" s="1" t="n">
         <v>845</v>
       </c>
-      <c r="H33" s="1" t="n">
+      <c r="J33" s="1" t="n">
+        <v>538</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>1241</v>
+      </c>
+      <c r="L33" s="1" t="n">
         <v>686</v>
       </c>
-      <c r="I33" s="1" t="n">
+      <c r="M33" s="1" t="n">
         <v>974</v>
       </c>
     </row>
@@ -983,22 +1043,22 @@
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="D34" s="1" t="n">
-        <v>543</v>
-      </c>
-      <c r="E34" s="1" t="n">
-        <v>1220</v>
-      </c>
       <c r="F34" s="1" t="n">
         <v>536</v>
       </c>
       <c r="G34" s="1" t="n">
         <v>826</v>
       </c>
-      <c r="H34" s="1" t="n">
+      <c r="J34" s="1" t="n">
+        <v>543</v>
+      </c>
+      <c r="K34" s="1" t="n">
+        <v>1220</v>
+      </c>
+      <c r="L34" s="1" t="n">
         <v>693</v>
       </c>
-      <c r="I34" s="1" t="n">
+      <c r="M34" s="1" t="n">
         <v>1008</v>
       </c>
     </row>
@@ -1006,22 +1066,22 @@
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="D35" s="1" t="n">
-        <v>553</v>
-      </c>
-      <c r="E35" s="1" t="n">
-        <v>1199</v>
-      </c>
       <c r="F35" s="1" t="n">
         <v>532</v>
       </c>
       <c r="G35" s="1" t="n">
         <v>826</v>
       </c>
-      <c r="H35" s="1" t="n">
+      <c r="J35" s="1" t="n">
+        <v>553</v>
+      </c>
+      <c r="K35" s="1" t="n">
+        <v>1199</v>
+      </c>
+      <c r="L35" s="1" t="n">
         <v>701</v>
       </c>
-      <c r="I35" s="1" t="n">
+      <c r="M35" s="1" t="n">
         <v>1037</v>
       </c>
     </row>
@@ -1029,22 +1089,22 @@
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D36" s="1" t="n">
-        <v>564</v>
-      </c>
-      <c r="E36" s="1" t="n">
-        <v>1183</v>
-      </c>
       <c r="F36" s="1" t="n">
         <v>526</v>
       </c>
       <c r="G36" s="1" t="n">
         <v>835</v>
       </c>
-      <c r="H36" s="1" t="n">
+      <c r="J36" s="1" t="n">
+        <v>564</v>
+      </c>
+      <c r="K36" s="1" t="n">
+        <v>1183</v>
+      </c>
+      <c r="L36" s="1" t="n">
         <v>707</v>
       </c>
-      <c r="I36" s="1" t="n">
+      <c r="M36" s="1" t="n">
         <v>1057</v>
       </c>
     </row>
@@ -1052,22 +1112,22 @@
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="D37" s="1" t="n">
-        <v>574</v>
-      </c>
-      <c r="E37" s="1" t="n">
-        <v>1157</v>
-      </c>
       <c r="F37" s="1" t="n">
         <v>521</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>823</v>
       </c>
-      <c r="H37" s="1" t="n">
+      <c r="J37" s="1" t="n">
+        <v>574</v>
+      </c>
+      <c r="K37" s="1" t="n">
+        <v>1157</v>
+      </c>
+      <c r="L37" s="1" t="n">
         <v>708</v>
       </c>
-      <c r="I37" s="1" t="n">
+      <c r="M37" s="1" t="n">
         <v>1073</v>
       </c>
     </row>
@@ -1075,22 +1135,22 @@
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="D38" s="1" t="n">
-        <v>590</v>
-      </c>
-      <c r="E38" s="1" t="n">
-        <v>1103</v>
-      </c>
       <c r="F38" s="1" t="n">
         <v>513</v>
       </c>
       <c r="G38" s="1" t="n">
         <v>830</v>
       </c>
-      <c r="H38" s="1" t="n">
+      <c r="J38" s="1" t="n">
+        <v>590</v>
+      </c>
+      <c r="K38" s="1" t="n">
+        <v>1103</v>
+      </c>
+      <c r="L38" s="1" t="n">
         <v>712</v>
       </c>
-      <c r="I38" s="1" t="n">
+      <c r="M38" s="1" t="n">
         <v>1093</v>
       </c>
     </row>
@@ -1098,22 +1158,22 @@
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="D39" s="1" t="n">
-        <v>595</v>
-      </c>
-      <c r="E39" s="1" t="n">
-        <v>1038</v>
-      </c>
       <c r="F39" s="1" t="n">
         <v>505</v>
       </c>
       <c r="G39" s="1" t="n">
         <v>839</v>
       </c>
-      <c r="H39" s="1" t="n">
+      <c r="J39" s="1" t="n">
+        <v>595</v>
+      </c>
+      <c r="K39" s="1" t="n">
+        <v>1038</v>
+      </c>
+      <c r="L39" s="1" t="n">
         <v>709</v>
       </c>
-      <c r="I39" s="1" t="n">
+      <c r="M39" s="1" t="n">
         <v>1116</v>
       </c>
     </row>
@@ -1121,22 +1181,22 @@
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="D40" s="1" t="n">
-        <v>596</v>
-      </c>
-      <c r="E40" s="1" t="n">
-        <v>983</v>
-      </c>
       <c r="F40" s="1" t="n">
         <v>501</v>
       </c>
       <c r="G40" s="1" t="n">
         <v>856</v>
       </c>
-      <c r="H40" s="1" t="n">
+      <c r="J40" s="1" t="n">
+        <v>596</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <v>983</v>
+      </c>
+      <c r="L40" s="1" t="n">
         <v>694</v>
       </c>
-      <c r="I40" s="1" t="n">
+      <c r="M40" s="1" t="n">
         <v>1136</v>
       </c>
     </row>
@@ -1144,22 +1204,22 @@
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="D41" s="1" t="n">
-        <v>596</v>
-      </c>
-      <c r="E41" s="1" t="n">
-        <v>936</v>
-      </c>
       <c r="F41" s="1" t="n">
         <v>500</v>
       </c>
       <c r="G41" s="1" t="n">
         <v>881</v>
       </c>
-      <c r="H41" s="1" t="n">
+      <c r="J41" s="1" t="n">
+        <v>596</v>
+      </c>
+      <c r="K41" s="1" t="n">
+        <v>936</v>
+      </c>
+      <c r="L41" s="1" t="n">
         <v>681</v>
       </c>
-      <c r="I41" s="1" t="n">
+      <c r="M41" s="1" t="n">
         <v>1155</v>
       </c>
     </row>
@@ -1167,22 +1227,22 @@
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="D42" s="1" t="n">
-        <v>594</v>
-      </c>
-      <c r="E42" s="1" t="n">
-        <v>892</v>
-      </c>
       <c r="F42" s="1" t="n">
         <v>498</v>
       </c>
       <c r="G42" s="1" t="n">
         <v>908</v>
       </c>
-      <c r="H42" s="1" t="n">
+      <c r="J42" s="1" t="n">
+        <v>594</v>
+      </c>
+      <c r="K42" s="1" t="n">
+        <v>892</v>
+      </c>
+      <c r="L42" s="1" t="n">
         <v>671</v>
       </c>
-      <c r="I42" s="1" t="n">
+      <c r="M42" s="1" t="n">
         <v>1172</v>
       </c>
     </row>
@@ -1190,22 +1250,22 @@
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="D43" s="1" t="n">
-        <v>592</v>
-      </c>
-      <c r="E43" s="1" t="n">
-        <v>862</v>
-      </c>
       <c r="F43" s="1" t="n">
         <v>495</v>
       </c>
       <c r="G43" s="1" t="n">
         <v>938</v>
       </c>
-      <c r="H43" s="1" t="n">
+      <c r="J43" s="1" t="n">
+        <v>592</v>
+      </c>
+      <c r="K43" s="1" t="n">
+        <v>862</v>
+      </c>
+      <c r="L43" s="1" t="n">
         <v>664</v>
       </c>
-      <c r="I43" s="1" t="n">
+      <c r="M43" s="1" t="n">
         <v>1190</v>
       </c>
     </row>
@@ -1213,22 +1273,22 @@
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="D44" s="1" t="n">
-        <v>593</v>
-      </c>
-      <c r="E44" s="1" t="n">
-        <v>832</v>
-      </c>
       <c r="F44" s="1" t="n">
         <v>492</v>
       </c>
       <c r="G44" s="1" t="n">
         <v>970</v>
       </c>
-      <c r="H44" s="1" t="n">
+      <c r="J44" s="1" t="n">
+        <v>593</v>
+      </c>
+      <c r="K44" s="1" t="n">
+        <v>832</v>
+      </c>
+      <c r="L44" s="1" t="n">
         <v>659</v>
       </c>
-      <c r="I44" s="1" t="n">
+      <c r="M44" s="1" t="n">
         <v>1206</v>
       </c>
     </row>
@@ -1236,22 +1296,22 @@
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="D45" s="1" t="n">
-        <v>599</v>
-      </c>
-      <c r="E45" s="1" t="n">
-        <v>803</v>
-      </c>
       <c r="F45" s="1" t="n">
         <v>490</v>
       </c>
       <c r="G45" s="1" t="n">
         <v>1004</v>
       </c>
-      <c r="H45" s="1" t="n">
+      <c r="J45" s="1" t="n">
+        <v>599</v>
+      </c>
+      <c r="K45" s="1" t="n">
+        <v>803</v>
+      </c>
+      <c r="L45" s="1" t="n">
         <v>655</v>
       </c>
-      <c r="I45" s="1" t="n">
+      <c r="M45" s="1" t="n">
         <v>1215</v>
       </c>
     </row>
@@ -1259,22 +1319,22 @@
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="D46" s="1" t="n">
-        <v>603</v>
-      </c>
-      <c r="E46" s="1" t="n">
-        <v>785</v>
-      </c>
       <c r="F46" s="1" t="n">
         <v>489</v>
       </c>
       <c r="G46" s="1" t="n">
         <v>1030</v>
       </c>
-      <c r="H46" s="1" t="n">
+      <c r="J46" s="1" t="n">
+        <v>603</v>
+      </c>
+      <c r="K46" s="1" t="n">
+        <v>785</v>
+      </c>
+      <c r="L46" s="1" t="n">
         <v>647</v>
       </c>
-      <c r="I46" s="1" t="n">
+      <c r="M46" s="1" t="n">
         <v>1217</v>
       </c>
     </row>
@@ -1282,22 +1342,22 @@
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="D47" s="1" t="n">
-        <v>607</v>
-      </c>
-      <c r="E47" s="1" t="n">
-        <v>769</v>
-      </c>
       <c r="F47" s="1" t="n">
         <v>482</v>
       </c>
       <c r="G47" s="1" t="n">
         <v>1051</v>
       </c>
-      <c r="H47" s="1" t="n">
+      <c r="J47" s="1" t="n">
+        <v>607</v>
+      </c>
+      <c r="K47" s="1" t="n">
+        <v>769</v>
+      </c>
+      <c r="L47" s="1" t="n">
         <v>644</v>
       </c>
-      <c r="I47" s="1" t="n">
+      <c r="M47" s="1" t="n">
         <v>1223</v>
       </c>
     </row>
@@ -1305,22 +1365,22 @@
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="D48" s="1" t="n">
-        <v>610</v>
-      </c>
-      <c r="E48" s="1" t="n">
-        <v>754</v>
-      </c>
       <c r="F48" s="1" t="n">
         <v>480</v>
       </c>
       <c r="G48" s="1" t="n">
         <v>1062</v>
       </c>
-      <c r="H48" s="1" t="n">
+      <c r="J48" s="1" t="n">
+        <v>610</v>
+      </c>
+      <c r="K48" s="1" t="n">
+        <v>754</v>
+      </c>
+      <c r="L48" s="1" t="n">
         <v>635</v>
       </c>
-      <c r="I48" s="1" t="n">
+      <c r="M48" s="1" t="n">
         <v>1222</v>
       </c>
     </row>
@@ -1328,22 +1388,22 @@
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="D49" s="1" t="n">
-        <v>612</v>
-      </c>
-      <c r="E49" s="1" t="n">
-        <v>754</v>
-      </c>
       <c r="F49" s="1" t="n">
         <v>479</v>
       </c>
       <c r="G49" s="1" t="n">
         <v>1070</v>
       </c>
-      <c r="H49" s="1" t="n">
+      <c r="J49" s="1" t="n">
+        <v>612</v>
+      </c>
+      <c r="K49" s="1" t="n">
+        <v>754</v>
+      </c>
+      <c r="L49" s="1" t="n">
         <v>621</v>
       </c>
-      <c r="I49" s="1" t="n">
+      <c r="M49" s="1" t="n">
         <v>1197</v>
       </c>
     </row>
@@ -1351,22 +1411,22 @@
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="D50" s="1" t="n">
-        <v>615</v>
-      </c>
-      <c r="E50" s="1" t="n">
-        <v>763</v>
-      </c>
       <c r="F50" s="1" t="n">
         <v>479</v>
       </c>
       <c r="G50" s="1" t="n">
         <v>1084</v>
       </c>
-      <c r="H50" s="1" t="n">
+      <c r="J50" s="1" t="n">
+        <v>615</v>
+      </c>
+      <c r="K50" s="1" t="n">
+        <v>763</v>
+      </c>
+      <c r="L50" s="1" t="n">
         <v>606</v>
       </c>
-      <c r="I50" s="1" t="n">
+      <c r="M50" s="1" t="n">
         <v>1162</v>
       </c>
     </row>
@@ -1374,22 +1434,22 @@
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="D51" s="1" t="n">
-        <v>620</v>
-      </c>
-      <c r="E51" s="1" t="n">
-        <v>777</v>
-      </c>
       <c r="F51" s="1" t="n">
         <v>479</v>
       </c>
       <c r="G51" s="1" t="n">
         <v>1100</v>
       </c>
-      <c r="H51" s="1" t="n">
+      <c r="J51" s="1" t="n">
+        <v>620</v>
+      </c>
+      <c r="K51" s="1" t="n">
+        <v>777</v>
+      </c>
+      <c r="L51" s="1" t="n">
         <v>598</v>
       </c>
-      <c r="I51" s="1" t="n">
+      <c r="M51" s="1" t="n">
         <v>1136</v>
       </c>
     </row>
@@ -1397,22 +1457,22 @@
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="D52" s="1" t="n">
-        <v>626</v>
-      </c>
-      <c r="E52" s="1" t="n">
-        <v>792</v>
-      </c>
       <c r="F52" s="1" t="n">
         <v>487</v>
       </c>
       <c r="G52" s="1" t="n">
         <v>1117</v>
       </c>
-      <c r="H52" s="1" t="n">
+      <c r="J52" s="1" t="n">
+        <v>626</v>
+      </c>
+      <c r="K52" s="1" t="n">
+        <v>792</v>
+      </c>
+      <c r="L52" s="1" t="n">
         <v>588</v>
       </c>
-      <c r="I52" s="1" t="n">
+      <c r="M52" s="1" t="n">
         <v>1095</v>
       </c>
     </row>
@@ -1420,22 +1480,22 @@
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="D53" s="1" t="n">
-        <v>628</v>
-      </c>
-      <c r="E53" s="1" t="n">
-        <v>809</v>
-      </c>
       <c r="F53" s="1" t="n">
         <v>492</v>
       </c>
       <c r="G53" s="1" t="n">
         <v>1142</v>
       </c>
-      <c r="H53" s="1" t="n">
+      <c r="J53" s="1" t="n">
+        <v>628</v>
+      </c>
+      <c r="K53" s="1" t="n">
+        <v>809</v>
+      </c>
+      <c r="L53" s="1" t="n">
         <v>583</v>
       </c>
-      <c r="I53" s="1" t="n">
+      <c r="M53" s="1" t="n">
         <v>1042</v>
       </c>
     </row>
@@ -1443,22 +1503,22 @@
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D54" s="1" t="n">
-        <v>629</v>
-      </c>
-      <c r="E54" s="1" t="n">
-        <v>830</v>
-      </c>
       <c r="F54" s="1" t="n">
         <v>497</v>
       </c>
       <c r="G54" s="1" t="n">
         <v>1167</v>
       </c>
-      <c r="H54" s="1" t="n">
+      <c r="J54" s="1" t="n">
+        <v>629</v>
+      </c>
+      <c r="K54" s="1" t="n">
+        <v>830</v>
+      </c>
+      <c r="L54" s="1" t="n">
         <v>578</v>
       </c>
-      <c r="I54" s="1" t="n">
+      <c r="M54" s="1" t="n">
         <v>989</v>
       </c>
     </row>
@@ -1466,22 +1526,22 @@
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="D55" s="1" t="n">
-        <v>632</v>
-      </c>
-      <c r="E55" s="1" t="n">
-        <v>854</v>
-      </c>
       <c r="F55" s="1" t="n">
         <v>504</v>
       </c>
       <c r="G55" s="1" t="n">
         <v>1182</v>
       </c>
-      <c r="H55" s="1" t="n">
+      <c r="J55" s="1" t="n">
+        <v>632</v>
+      </c>
+      <c r="K55" s="1" t="n">
+        <v>854</v>
+      </c>
+      <c r="L55" s="1" t="n">
         <v>573</v>
       </c>
-      <c r="I55" s="1" t="n">
+      <c r="M55" s="1" t="n">
         <v>939</v>
       </c>
     </row>
@@ -1489,22 +1549,22 @@
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="D56" s="1" t="n">
-        <v>638</v>
-      </c>
-      <c r="E56" s="1" t="n">
-        <v>883</v>
-      </c>
       <c r="F56" s="1" t="n">
         <v>501</v>
       </c>
       <c r="G56" s="1" t="n">
         <v>1201</v>
       </c>
-      <c r="H56" s="1" t="n">
+      <c r="J56" s="1" t="n">
+        <v>638</v>
+      </c>
+      <c r="K56" s="1" t="n">
+        <v>883</v>
+      </c>
+      <c r="L56" s="1" t="n">
         <v>569</v>
       </c>
-      <c r="I56" s="1" t="n">
+      <c r="M56" s="1" t="n">
         <v>902</v>
       </c>
     </row>
@@ -1512,22 +1572,22 @@
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="D57" s="1" t="n">
-        <v>642</v>
-      </c>
-      <c r="E57" s="1" t="n">
-        <v>926</v>
-      </c>
       <c r="F57" s="1" t="n">
         <v>501</v>
       </c>
       <c r="G57" s="1" t="n">
         <v>1222</v>
       </c>
-      <c r="H57" s="1" t="n">
+      <c r="J57" s="1" t="n">
+        <v>642</v>
+      </c>
+      <c r="K57" s="1" t="n">
+        <v>926</v>
+      </c>
+      <c r="L57" s="1" t="n">
         <v>565</v>
       </c>
-      <c r="I57" s="1" t="n">
+      <c r="M57" s="1" t="n">
         <v>882</v>
       </c>
     </row>
@@ -1535,22 +1595,22 @@
       <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="D58" s="1" t="n">
-        <v>649</v>
-      </c>
-      <c r="E58" s="1" t="n">
-        <v>964</v>
-      </c>
       <c r="F58" s="1" t="n">
         <v>504</v>
       </c>
       <c r="G58" s="1" t="n">
         <v>1241</v>
       </c>
-      <c r="H58" s="1" t="n">
+      <c r="J58" s="1" t="n">
+        <v>649</v>
+      </c>
+      <c r="K58" s="1" t="n">
+        <v>964</v>
+      </c>
+      <c r="L58" s="1" t="n">
         <v>560</v>
       </c>
-      <c r="I58" s="1" t="n">
+      <c r="M58" s="1" t="n">
         <v>862</v>
       </c>
     </row>
@@ -1558,22 +1618,22 @@
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="D59" s="1" t="n">
-        <v>658</v>
-      </c>
-      <c r="E59" s="1" t="n">
-        <v>985</v>
-      </c>
       <c r="F59" s="1" t="n">
         <v>509</v>
       </c>
       <c r="G59" s="1" t="n">
         <v>1249</v>
       </c>
-      <c r="H59" s="1" t="n">
+      <c r="J59" s="1" t="n">
+        <v>658</v>
+      </c>
+      <c r="K59" s="1" t="n">
+        <v>985</v>
+      </c>
+      <c r="L59" s="1" t="n">
         <v>554</v>
       </c>
-      <c r="I59" s="1" t="n">
+      <c r="M59" s="1" t="n">
         <v>838</v>
       </c>
     </row>
@@ -1581,22 +1641,22 @@
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="D60" s="1" t="n">
-        <v>666</v>
-      </c>
-      <c r="E60" s="1" t="n">
-        <v>989</v>
-      </c>
       <c r="F60" s="1" t="n">
         <v>517</v>
       </c>
       <c r="G60" s="1" t="n">
         <v>1234</v>
       </c>
-      <c r="H60" s="1" t="n">
+      <c r="J60" s="1" t="n">
+        <v>666</v>
+      </c>
+      <c r="K60" s="1" t="n">
+        <v>989</v>
+      </c>
+      <c r="L60" s="1" t="n">
         <v>548</v>
       </c>
-      <c r="I60" s="1" t="n">
+      <c r="M60" s="1" t="n">
         <v>814</v>
       </c>
     </row>
@@ -1604,22 +1664,22 @@
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="D61" s="1" t="n">
-        <v>673</v>
-      </c>
-      <c r="E61" s="1" t="n">
-        <v>1000</v>
-      </c>
       <c r="F61" s="1" t="n">
         <v>530</v>
       </c>
       <c r="G61" s="1" t="n">
         <v>1218</v>
       </c>
-      <c r="H61" s="1" t="n">
+      <c r="J61" s="1" t="n">
+        <v>673</v>
+      </c>
+      <c r="K61" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L61" s="1" t="n">
         <v>546</v>
       </c>
-      <c r="I61" s="1" t="n">
+      <c r="M61" s="1" t="n">
         <v>797</v>
       </c>
     </row>
@@ -1627,22 +1687,22 @@
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D62" s="1" t="n">
-        <v>680</v>
-      </c>
-      <c r="E62" s="1" t="n">
-        <v>1011</v>
-      </c>
       <c r="F62" s="1" t="n">
         <v>546</v>
       </c>
       <c r="G62" s="1" t="n">
         <v>1201</v>
       </c>
-      <c r="H62" s="1" t="n">
+      <c r="J62" s="1" t="n">
+        <v>680</v>
+      </c>
+      <c r="K62" s="1" t="n">
+        <v>1011</v>
+      </c>
+      <c r="L62" s="1" t="n">
         <v>542</v>
       </c>
-      <c r="I62" s="1" t="n">
+      <c r="M62" s="1" t="n">
         <v>788</v>
       </c>
     </row>
@@ -1650,22 +1710,22 @@
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="D63" s="1" t="n">
-        <v>687</v>
-      </c>
-      <c r="E63" s="1" t="n">
-        <v>1024</v>
-      </c>
       <c r="F63" s="1" t="n">
         <v>567</v>
       </c>
       <c r="G63" s="1" t="n">
         <v>1180</v>
       </c>
-      <c r="H63" s="1" t="n">
+      <c r="J63" s="1" t="n">
+        <v>687</v>
+      </c>
+      <c r="K63" s="1" t="n">
+        <v>1024</v>
+      </c>
+      <c r="L63" s="1" t="n">
         <v>536</v>
       </c>
-      <c r="I63" s="1" t="n">
+      <c r="M63" s="1" t="n">
         <v>793</v>
       </c>
     </row>
@@ -1673,22 +1733,22 @@
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="D64" s="1" t="n">
-        <v>691</v>
-      </c>
-      <c r="E64" s="1" t="n">
-        <v>1044</v>
-      </c>
       <c r="F64" s="1" t="n">
         <v>588</v>
       </c>
       <c r="G64" s="1" t="n">
         <v>1156</v>
       </c>
-      <c r="H64" s="1" t="n">
+      <c r="J64" s="1" t="n">
+        <v>691</v>
+      </c>
+      <c r="K64" s="1" t="n">
+        <v>1044</v>
+      </c>
+      <c r="L64" s="1" t="n">
         <v>530</v>
       </c>
-      <c r="I64" s="1" t="n">
+      <c r="M64" s="1" t="n">
         <v>802</v>
       </c>
     </row>
@@ -1696,22 +1756,22 @@
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="D65" s="1" t="n">
-        <v>695</v>
-      </c>
-      <c r="E65" s="1" t="n">
-        <v>1065</v>
-      </c>
       <c r="F65" s="1" t="n">
         <v>594</v>
       </c>
       <c r="G65" s="1" t="n">
         <v>1102</v>
       </c>
-      <c r="H65" s="1" t="n">
+      <c r="J65" s="1" t="n">
+        <v>695</v>
+      </c>
+      <c r="K65" s="1" t="n">
+        <v>1065</v>
+      </c>
+      <c r="L65" s="1" t="n">
         <v>527</v>
       </c>
-      <c r="I65" s="1" t="n">
+      <c r="M65" s="1" t="n">
         <v>816</v>
       </c>
     </row>
@@ -1719,22 +1779,22 @@
       <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="D66" s="1" t="n">
-        <v>699</v>
-      </c>
-      <c r="E66" s="1" t="n">
-        <v>1089</v>
-      </c>
       <c r="F66" s="1" t="n">
         <v>595</v>
       </c>
       <c r="G66" s="1" t="n">
         <v>1038</v>
       </c>
-      <c r="H66" s="1" t="n">
+      <c r="J66" s="1" t="n">
+        <v>699</v>
+      </c>
+      <c r="K66" s="1" t="n">
+        <v>1089</v>
+      </c>
+      <c r="L66" s="1" t="n">
         <v>524</v>
       </c>
-      <c r="I66" s="1" t="n">
+      <c r="M66" s="1" t="n">
         <v>835</v>
       </c>
     </row>
@@ -1742,22 +1802,22 @@
       <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="D67" s="1" t="n">
-        <v>701</v>
-      </c>
-      <c r="E67" s="1" t="n">
-        <v>1115</v>
-      </c>
       <c r="F67" s="1" t="n">
         <v>597</v>
       </c>
       <c r="G67" s="1" t="n">
         <v>970</v>
       </c>
-      <c r="H67" s="1" t="n">
+      <c r="J67" s="1" t="n">
+        <v>701</v>
+      </c>
+      <c r="K67" s="1" t="n">
+        <v>1115</v>
+      </c>
+      <c r="L67" s="1" t="n">
         <v>522</v>
       </c>
-      <c r="I67" s="1" t="n">
+      <c r="M67" s="1" t="n">
         <v>858</v>
       </c>
     </row>
@@ -1765,32 +1825,35 @@
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="D68" s="1" t="n">
-        <v>700</v>
-      </c>
-      <c r="E68" s="1" t="n">
-        <v>1142</v>
-      </c>
       <c r="F68" s="1" t="n">
         <v>600</v>
       </c>
       <c r="G68" s="1" t="n">
         <v>924</v>
       </c>
-      <c r="H68" s="1" t="n">
+      <c r="J68" s="1" t="n">
+        <v>700</v>
+      </c>
+      <c r="K68" s="1" t="n">
+        <v>1142</v>
+      </c>
+      <c r="L68" s="1" t="n">
         <v>519</v>
       </c>
-      <c r="I68" s="1" t="n">
+      <c r="M68" s="1" t="n">
         <v>885</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>